<commit_message>
Refactor roster loading logic to improve CSV parsing and enhance player display formatting; update roster rendering in DOM.
</commit_message>
<xml_diff>
--- a/templates/rosters.xlsx
+++ b/templates/rosters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c420bd46a5738fd/Documents/GitHub/nbcml/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{98E44900-1AF4-41E7-83DA-86A15D56D0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{158C40E4-0AAA-424B-BE88-31691C91EA8A}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{98E44900-1AF4-41E7-83DA-86A15D56D0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A36231D-7661-4525-A0E4-E95358C84D70}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9077D6FF-DD53-4FA0-A1AB-BC2E9F42BF0A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="154">
   <si>
     <t>Team</t>
   </si>
@@ -477,24 +477,37 @@
   </si>
   <si>
     <t>rick@email.com</t>
+  </si>
+  <si>
+    <t>GamesPlayed</t>
+  </si>
+  <si>
+    <t>TotalPts</t>
+  </si>
+  <si>
+    <t>PPG</t>
+  </si>
+  <si>
+    <t>TotalFouls</t>
+  </si>
+  <si>
+    <t>FPG</t>
+  </si>
+  <si>
+    <t>TotalTechs</t>
+  </si>
+  <si>
+    <t>TPG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -523,16 +536,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -865,10 +876,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B089AB-C826-4619-B243-5B13AFD7DC37}">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:K1048576"/>
+      <selection activeCell="F2" sqref="F2:F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -879,7 +890,7 @@
     <col min="6" max="6" width="18.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -898,8 +909,29 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H1" t="s">
+        <v>148</v>
+      </c>
+      <c r="I1" t="s">
+        <v>149</v>
+      </c>
+      <c r="J1" t="s">
+        <v>150</v>
+      </c>
+      <c r="K1" t="s">
+        <v>151</v>
+      </c>
+      <c r="L1" t="s">
+        <v>152</v>
+      </c>
+      <c r="M1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -916,7 +948,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -933,7 +965,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -950,7 +982,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -967,7 +999,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -984,7 +1016,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1001,7 +1033,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1018,7 +1050,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1035,7 +1067,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1052,7 +1084,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1069,7 +1101,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1086,7 +1118,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1103,7 +1135,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -1120,7 +1152,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1137,7 +1169,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1716,58 +1748,8 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{E13ABAE0-ADA0-4571-9085-0968C29C0C19}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{F568EF93-1CAD-4E66-B7F7-D3B19202059E}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{B66855BB-2684-44ED-861A-6124C764F09C}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{1F40441D-C868-4098-83BC-0F535B207EA7}"/>
-    <hyperlink ref="F6" r:id="rId5" xr:uid="{4E40BF87-C4AB-416F-A9DE-D3EDD6BDA8BC}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{BD568C25-8909-47CD-8159-080635F22B06}"/>
-    <hyperlink ref="F8" r:id="rId7" xr:uid="{8C4E3A3D-1AD1-45E5-BF02-7952BD25FD5C}"/>
-    <hyperlink ref="F9" r:id="rId8" xr:uid="{DFB5FBCC-9DEB-497A-8536-280B17BF5D89}"/>
-    <hyperlink ref="F10" r:id="rId9" xr:uid="{77DC068D-9507-4C8C-8394-9290B3AC3E54}"/>
-    <hyperlink ref="F11" r:id="rId10" xr:uid="{229B0F7F-53A4-421F-830C-50136603BF81}"/>
-    <hyperlink ref="F12" r:id="rId11" xr:uid="{85D45D6D-8781-4E5B-819E-B59B57DAF0E7}"/>
-    <hyperlink ref="F13" r:id="rId12" xr:uid="{CB89572D-0498-41A8-A978-C99DE2A66839}"/>
-    <hyperlink ref="F14" r:id="rId13" xr:uid="{87C3BC58-BC54-4C11-A2F4-1F09B86A3996}"/>
-    <hyperlink ref="F15" r:id="rId14" xr:uid="{2C3D6F56-CF4A-4E06-B72F-61D9ABF565A8}"/>
-    <hyperlink ref="F16" r:id="rId15" xr:uid="{B092DCB8-CD24-442C-AD22-892362DAAC44}"/>
-    <hyperlink ref="F17" r:id="rId16" xr:uid="{452A9753-F914-4AD2-A689-C9C465B3AC65}"/>
-    <hyperlink ref="F18" r:id="rId17" xr:uid="{7C581034-8637-4090-AFBB-5AD08472531C}"/>
-    <hyperlink ref="F19" r:id="rId18" xr:uid="{3BCADB75-2304-49AE-BE1C-6B200354CE96}"/>
-    <hyperlink ref="F20" r:id="rId19" xr:uid="{BD0DDAEE-9762-4594-94EF-29F0B96A0830}"/>
-    <hyperlink ref="F21" r:id="rId20" xr:uid="{212F43AF-0189-4AB9-83B3-5E61D2F4DBBF}"/>
-    <hyperlink ref="F22" r:id="rId21" xr:uid="{8E50FDA9-7A83-4182-A009-3281622DB4F0}"/>
-    <hyperlink ref="F23" r:id="rId22" xr:uid="{2E1C1BE1-1F99-4E36-89DB-C3B875C33DCE}"/>
-    <hyperlink ref="F24" r:id="rId23" xr:uid="{68C78885-2DB5-4AEE-A22D-1752639735CA}"/>
-    <hyperlink ref="F25" r:id="rId24" xr:uid="{9E189CA4-25C2-4074-939D-08BFE08F8E3E}"/>
-    <hyperlink ref="F26" r:id="rId25" xr:uid="{F8E80004-27D3-4E52-9496-91FCD70E9A30}"/>
-    <hyperlink ref="F27" r:id="rId26" xr:uid="{C0B7E321-A4A6-43E3-A3F2-ACBC4CF31131}"/>
-    <hyperlink ref="F28" r:id="rId27" xr:uid="{87E759A2-606F-4A54-9E9E-296E9E6F2AA8}"/>
-    <hyperlink ref="F29" r:id="rId28" xr:uid="{6BD6D67E-E9E8-4231-B80F-8CB6E8F778F1}"/>
-    <hyperlink ref="F30" r:id="rId29" xr:uid="{F7852C6D-06D6-4B41-92B0-85FA67371723}"/>
-    <hyperlink ref="F31" r:id="rId30" xr:uid="{7A234696-298B-40B4-8D74-768D738523F3}"/>
-    <hyperlink ref="F32" r:id="rId31" xr:uid="{965FF6FE-FBE6-45BC-8212-6685C99B22C6}"/>
-    <hyperlink ref="F33" r:id="rId32" xr:uid="{D147DFA4-B51A-4F8A-85B5-B30A0208B6EE}"/>
-    <hyperlink ref="F34" r:id="rId33" xr:uid="{87F530B7-9FB1-46DA-85CB-E251BA2C7E23}"/>
-    <hyperlink ref="F35" r:id="rId34" xr:uid="{CF9002E8-42B9-4170-A296-99558EECDD75}"/>
-    <hyperlink ref="F36" r:id="rId35" xr:uid="{C6F9EAFD-7E37-44F8-8042-8D00559BB803}"/>
-    <hyperlink ref="F37" r:id="rId36" xr:uid="{6FCF174C-97C3-404B-807E-8A061C02C161}"/>
-    <hyperlink ref="F38" r:id="rId37" xr:uid="{1F0C6D3B-E9F0-405C-95AA-5BC26A95CA71}"/>
-    <hyperlink ref="F39" r:id="rId38" xr:uid="{FC69A1C7-A11F-48A3-81AE-3722C1294A3A}"/>
-    <hyperlink ref="F40" r:id="rId39" xr:uid="{EA1C7011-0AB6-41C7-BD5E-42ED10709D2B}"/>
-    <hyperlink ref="F41" r:id="rId40" xr:uid="{19E3CB48-D08A-40D7-9FDB-97989B572D0D}"/>
-    <hyperlink ref="F42" r:id="rId41" xr:uid="{55C906ED-BE01-4D1E-AAAE-CBAEC8376563}"/>
-    <hyperlink ref="F43" r:id="rId42" xr:uid="{F1773A22-A34D-4172-88E4-88F574B78BD9}"/>
-    <hyperlink ref="F44" r:id="rId43" xr:uid="{1D88EAC9-C05C-4BDA-A7CA-ED1132188D09}"/>
-    <hyperlink ref="F45" r:id="rId44" xr:uid="{7520F5C5-D384-41CA-B3A0-B6EDFB63E9E9}"/>
-    <hyperlink ref="F46" r:id="rId45" xr:uid="{0322FB61-9B99-427B-BC20-8FCD190EFA2E}"/>
-    <hyperlink ref="F47" r:id="rId46" xr:uid="{0488E5EE-21EA-43CC-9794-CBBD7E333749}"/>
-    <hyperlink ref="F48" r:id="rId47" xr:uid="{375B9A41-A1A3-47FC-A26E-74905667F8C6}"/>
-    <hyperlink ref="F49" r:id="rId48" xr:uid="{9270A195-F7DA-4613-A3E4-0E7300936D96}"/>
-  </hyperlinks>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId49"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Enhance roster and player statistics functionality; update CSV structure, improve player stats calculation, and refine rendering styles for better display.
</commit_message>
<xml_diff>
--- a/templates/rosters.xlsx
+++ b/templates/rosters.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c420bd46a5738fd/Documents/GitHub/nbcml/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{98E44900-1AF4-41E7-83DA-86A15D56D0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A36231D-7661-4525-A0E4-E95358C84D70}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{98E44900-1AF4-41E7-83DA-86A15D56D0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11EA5999-4B5E-42F7-9AA8-5F69EAAA0225}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9077D6FF-DD53-4FA0-A1AB-BC2E9F42BF0A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="rosters" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="151">
   <si>
     <t>Team</t>
   </si>
@@ -485,19 +485,10 @@
     <t>TotalPts</t>
   </si>
   <si>
-    <t>PPG</t>
-  </si>
-  <si>
     <t>TotalFouls</t>
   </si>
   <si>
-    <t>FPG</t>
-  </si>
-  <si>
     <t>TotalTechs</t>
-  </si>
-  <si>
-    <t>TPG</t>
   </si>
 </sst>
 </file>
@@ -876,10 +867,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B089AB-C826-4619-B243-5B13AFD7DC37}">
-  <dimension ref="A1:M49"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F49"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -888,9 +879,11 @@
     <col min="2" max="2" width="9.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -921,17 +914,8 @@
       <c r="J1" t="s">
         <v>150</v>
       </c>
-      <c r="K1" t="s">
-        <v>151</v>
-      </c>
-      <c r="L1" t="s">
-        <v>152</v>
-      </c>
-      <c r="M1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -944,11 +928,26 @@
       <c r="D2" t="b">
         <v>1</v>
       </c>
+      <c r="E2">
+        <v>25</v>
+      </c>
       <c r="F2" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G2">
+        <v>25</v>
+      </c>
+      <c r="H2">
+        <v>712</v>
+      </c>
+      <c r="I2">
+        <v>75</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -964,8 +963,20 @@
       <c r="F3" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G3">
+        <v>19</v>
+      </c>
+      <c r="H3">
+        <v>514</v>
+      </c>
+      <c r="I3">
+        <v>11</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -978,11 +989,26 @@
       <c r="D4" t="b">
         <v>0</v>
       </c>
+      <c r="E4">
+        <v>18</v>
+      </c>
       <c r="F4" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G4">
+        <v>19</v>
+      </c>
+      <c r="H4">
+        <v>477</v>
+      </c>
+      <c r="I4">
+        <v>61</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -995,11 +1021,26 @@
       <c r="D5" t="b">
         <v>0</v>
       </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
       <c r="F5" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G5">
+        <v>16</v>
+      </c>
+      <c r="H5">
+        <v>360</v>
+      </c>
+      <c r="I5">
+        <v>43</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1012,11 +1053,26 @@
       <c r="D6" t="b">
         <v>0</v>
       </c>
+      <c r="E6">
+        <v>23</v>
+      </c>
       <c r="F6" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G6">
+        <v>25</v>
+      </c>
+      <c r="H6">
+        <v>520</v>
+      </c>
+      <c r="I6">
+        <v>9</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1029,11 +1085,26 @@
       <c r="D7" t="b">
         <v>0</v>
       </c>
+      <c r="E7">
+        <v>41</v>
+      </c>
       <c r="F7" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G7">
+        <v>27</v>
+      </c>
+      <c r="H7">
+        <v>555</v>
+      </c>
+      <c r="I7">
+        <v>65</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1046,11 +1117,26 @@
       <c r="D8" t="b">
         <v>0</v>
       </c>
+      <c r="E8">
+        <v>34</v>
+      </c>
       <c r="F8" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G8">
+        <v>27</v>
+      </c>
+      <c r="H8">
+        <v>535</v>
+      </c>
+      <c r="I8">
+        <v>55</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1063,11 +1149,26 @@
       <c r="D9" t="b">
         <v>0</v>
       </c>
+      <c r="E9">
+        <v>50</v>
+      </c>
       <c r="F9" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G9">
+        <v>28</v>
+      </c>
+      <c r="H9">
+        <v>533</v>
+      </c>
+      <c r="I9">
+        <v>76</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1080,11 +1181,26 @@
       <c r="D10" t="b">
         <v>0</v>
       </c>
+      <c r="E10">
+        <v>28</v>
+      </c>
       <c r="F10" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G10">
+        <v>27</v>
+      </c>
+      <c r="H10">
+        <v>505</v>
+      </c>
+      <c r="I10">
+        <v>35</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1097,11 +1213,26 @@
       <c r="D11" t="b">
         <v>0</v>
       </c>
+      <c r="E11">
+        <v>68</v>
+      </c>
       <c r="F11" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G11">
+        <v>14</v>
+      </c>
+      <c r="H11">
+        <v>249</v>
+      </c>
+      <c r="I11">
+        <v>68</v>
+      </c>
+      <c r="J11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1114,11 +1245,26 @@
       <c r="D12" t="b">
         <v>0</v>
       </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
       <c r="F12" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G12">
+        <v>22</v>
+      </c>
+      <c r="H12">
+        <v>390</v>
+      </c>
+      <c r="I12">
+        <v>6</v>
+      </c>
+      <c r="J12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1134,8 +1280,20 @@
       <c r="F13" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G13">
+        <v>21</v>
+      </c>
+      <c r="H13">
+        <v>334</v>
+      </c>
+      <c r="I13">
+        <v>12</v>
+      </c>
+      <c r="J13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -1148,11 +1306,26 @@
       <c r="D14" t="b">
         <v>1</v>
       </c>
+      <c r="E14">
+        <v>47</v>
+      </c>
       <c r="F14" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G14">
+        <v>23</v>
+      </c>
+      <c r="H14">
+        <v>352</v>
+      </c>
+      <c r="I14">
+        <v>43</v>
+      </c>
+      <c r="J14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1165,11 +1338,26 @@
       <c r="D15" t="b">
         <v>0</v>
       </c>
+      <c r="E15">
+        <v>27</v>
+      </c>
       <c r="F15" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G15">
+        <v>24</v>
+      </c>
+      <c r="H15">
+        <v>356</v>
+      </c>
+      <c r="I15">
+        <v>11</v>
+      </c>
+      <c r="J15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1182,11 +1370,26 @@
       <c r="D16" t="b">
         <v>0</v>
       </c>
+      <c r="E16">
+        <v>21</v>
+      </c>
       <c r="F16" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G16">
+        <v>15</v>
+      </c>
+      <c r="H16">
+        <v>199</v>
+      </c>
+      <c r="I16">
+        <v>51</v>
+      </c>
+      <c r="J16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1199,11 +1402,26 @@
       <c r="D17" t="b">
         <v>0</v>
       </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
       <c r="F17" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G17">
+        <v>19</v>
+      </c>
+      <c r="H17">
+        <v>252</v>
+      </c>
+      <c r="I17">
+        <v>40</v>
+      </c>
+      <c r="J17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>59</v>
       </c>
@@ -1216,11 +1434,26 @@
       <c r="D18" t="b">
         <v>0</v>
       </c>
+      <c r="E18">
+        <v>52</v>
+      </c>
       <c r="F18" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G18">
+        <v>20</v>
+      </c>
+      <c r="H18">
+        <v>264</v>
+      </c>
+      <c r="I18">
+        <v>71</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -1233,11 +1466,26 @@
       <c r="D19" t="b">
         <v>0</v>
       </c>
+      <c r="E19">
+        <v>6</v>
+      </c>
       <c r="F19" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G19">
+        <v>27</v>
+      </c>
+      <c r="H19">
+        <v>339</v>
+      </c>
+      <c r="I19">
+        <v>69</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -1250,11 +1498,26 @@
       <c r="D20" t="b">
         <v>0</v>
       </c>
+      <c r="E20">
+        <v>39</v>
+      </c>
       <c r="F20" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G20">
+        <v>21</v>
+      </c>
+      <c r="H20">
+        <v>252</v>
+      </c>
+      <c r="I20">
+        <v>53</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -1267,11 +1530,26 @@
       <c r="D21" t="b">
         <v>1</v>
       </c>
+      <c r="E21">
+        <v>16</v>
+      </c>
       <c r="F21" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G21">
+        <v>26</v>
+      </c>
+      <c r="H21">
+        <v>299</v>
+      </c>
+      <c r="I21">
+        <v>10</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -1284,11 +1562,26 @@
       <c r="D22" t="b">
         <v>0</v>
       </c>
+      <c r="E22">
+        <v>31</v>
+      </c>
       <c r="F22" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G22">
+        <v>13</v>
+      </c>
+      <c r="H22">
+        <v>149</v>
+      </c>
+      <c r="I22">
+        <v>15</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>59</v>
       </c>
@@ -1301,11 +1594,26 @@
       <c r="D23" t="b">
         <v>0</v>
       </c>
+      <c r="E23">
+        <v>57</v>
+      </c>
       <c r="F23" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G23">
+        <v>14</v>
+      </c>
+      <c r="H23">
+        <v>159</v>
+      </c>
+      <c r="I23">
+        <v>64</v>
+      </c>
+      <c r="J23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>59</v>
       </c>
@@ -1318,11 +1626,26 @@
       <c r="D24" t="b">
         <v>0</v>
       </c>
+      <c r="E24">
+        <v>7</v>
+      </c>
       <c r="F24" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G24">
+        <v>27</v>
+      </c>
+      <c r="H24">
+        <v>306</v>
+      </c>
+      <c r="I24">
+        <v>56</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -1335,11 +1658,26 @@
       <c r="D25" t="b">
         <v>0</v>
       </c>
+      <c r="E25">
+        <v>24</v>
+      </c>
       <c r="F25" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G25">
+        <v>24</v>
+      </c>
+      <c r="H25">
+        <v>249</v>
+      </c>
+      <c r="I25">
+        <v>73</v>
+      </c>
+      <c r="J25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>60</v>
       </c>
@@ -1352,11 +1690,26 @@
       <c r="D26" t="b">
         <v>0</v>
       </c>
+      <c r="E26">
+        <v>55</v>
+      </c>
       <c r="F26" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G26">
+        <v>16</v>
+      </c>
+      <c r="H26">
+        <v>162</v>
+      </c>
+      <c r="I26">
+        <v>10</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -1369,11 +1722,26 @@
       <c r="D27" t="b">
         <v>0</v>
       </c>
+      <c r="E27">
+        <v>33</v>
+      </c>
       <c r="F27" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G27">
+        <v>6</v>
+      </c>
+      <c r="H27">
+        <v>58</v>
+      </c>
+      <c r="I27">
+        <v>65</v>
+      </c>
+      <c r="J27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -1386,11 +1754,26 @@
       <c r="D28" t="b">
         <v>0</v>
       </c>
+      <c r="E28">
+        <v>11</v>
+      </c>
       <c r="F28" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G28">
+        <v>25</v>
+      </c>
+      <c r="H28">
+        <v>241</v>
+      </c>
+      <c r="I28">
+        <v>39</v>
+      </c>
+      <c r="J28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -1403,11 +1786,26 @@
       <c r="D29" t="b">
         <v>0</v>
       </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
       <c r="F29" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G29">
+        <v>17</v>
+      </c>
+      <c r="H29">
+        <v>142</v>
+      </c>
+      <c r="I29">
+        <v>59</v>
+      </c>
+      <c r="J29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>60</v>
       </c>
@@ -1420,11 +1818,26 @@
       <c r="D30" t="b">
         <v>0</v>
       </c>
+      <c r="E30">
+        <v>39</v>
+      </c>
       <c r="F30" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G30">
+        <v>21</v>
+      </c>
+      <c r="H30">
+        <v>173</v>
+      </c>
+      <c r="I30">
+        <v>26</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -1437,11 +1850,26 @@
       <c r="D31" t="b">
         <v>0</v>
       </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
       <c r="F31" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G31">
+        <v>19</v>
+      </c>
+      <c r="H31">
+        <v>148</v>
+      </c>
+      <c r="I31">
+        <v>71</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>60</v>
       </c>
@@ -1454,11 +1882,26 @@
       <c r="D32" t="b">
         <v>1</v>
       </c>
+      <c r="E32">
+        <v>42</v>
+      </c>
       <c r="F32" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G32">
+        <v>20</v>
+      </c>
+      <c r="H32">
+        <v>154</v>
+      </c>
+      <c r="I32">
+        <v>65</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>60</v>
       </c>
@@ -1471,11 +1914,26 @@
       <c r="D33" t="b">
         <v>0</v>
       </c>
+      <c r="E33">
+        <v>10</v>
+      </c>
       <c r="F33" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G33">
+        <v>25</v>
+      </c>
+      <c r="H33">
+        <v>184</v>
+      </c>
+      <c r="I33">
+        <v>28</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -1488,11 +1946,26 @@
       <c r="D34" t="b">
         <v>0</v>
       </c>
+      <c r="E34">
+        <v>37</v>
+      </c>
       <c r="F34" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G34">
+        <v>16</v>
+      </c>
+      <c r="H34">
+        <v>107</v>
+      </c>
+      <c r="I34">
+        <v>41</v>
+      </c>
+      <c r="J34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>61</v>
       </c>
@@ -1505,11 +1978,26 @@
       <c r="D35" t="b">
         <v>0</v>
       </c>
+      <c r="E35">
+        <v>30</v>
+      </c>
       <c r="F35" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G35">
+        <v>26</v>
+      </c>
+      <c r="H35">
+        <v>170</v>
+      </c>
+      <c r="I35">
+        <v>44</v>
+      </c>
+      <c r="J35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>61</v>
       </c>
@@ -1522,11 +2010,26 @@
       <c r="D36" t="b">
         <v>0</v>
       </c>
+      <c r="E36">
+        <v>55</v>
+      </c>
       <c r="F36" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G36">
+        <v>14</v>
+      </c>
+      <c r="H36">
+        <v>83</v>
+      </c>
+      <c r="I36">
+        <v>73</v>
+      </c>
+      <c r="J36">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>61</v>
       </c>
@@ -1539,11 +2042,26 @@
       <c r="D37" t="b">
         <v>0</v>
       </c>
+      <c r="E37">
+        <v>32</v>
+      </c>
       <c r="F37" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G37">
+        <v>23</v>
+      </c>
+      <c r="H37">
+        <v>135</v>
+      </c>
+      <c r="I37">
+        <v>26</v>
+      </c>
+      <c r="J37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>61</v>
       </c>
@@ -1556,11 +2074,26 @@
       <c r="D38" t="b">
         <v>1</v>
       </c>
+      <c r="E38">
+        <v>17</v>
+      </c>
       <c r="F38" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G38">
+        <v>24</v>
+      </c>
+      <c r="H38">
+        <v>137</v>
+      </c>
+      <c r="I38">
+        <v>66</v>
+      </c>
+      <c r="J38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>61</v>
       </c>
@@ -1573,11 +2106,26 @@
       <c r="D39" t="b">
         <v>0</v>
       </c>
+      <c r="E39">
+        <v>8</v>
+      </c>
       <c r="F39" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G39">
+        <v>23</v>
+      </c>
+      <c r="H39">
+        <v>109</v>
+      </c>
+      <c r="I39">
+        <v>79</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>61</v>
       </c>
@@ -1590,11 +2138,26 @@
       <c r="D40" t="b">
         <v>0</v>
       </c>
+      <c r="E40">
+        <v>32</v>
+      </c>
       <c r="F40" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G40">
+        <v>12</v>
+      </c>
+      <c r="H40">
+        <v>55</v>
+      </c>
+      <c r="I40">
+        <v>50</v>
+      </c>
+      <c r="J40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>61</v>
       </c>
@@ -1607,11 +2170,26 @@
       <c r="D41" t="b">
         <v>0</v>
       </c>
+      <c r="E41">
+        <v>26</v>
+      </c>
       <c r="F41" s="1" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G41">
+        <v>17</v>
+      </c>
+      <c r="H41">
+        <v>76</v>
+      </c>
+      <c r="I41">
+        <v>8</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>62</v>
       </c>
@@ -1624,11 +2202,26 @@
       <c r="D42" t="b">
         <v>0</v>
       </c>
+      <c r="E42">
+        <v>14</v>
+      </c>
       <c r="F42" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G42">
+        <v>28</v>
+      </c>
+      <c r="H42">
+        <v>125</v>
+      </c>
+      <c r="I42">
+        <v>45</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>62</v>
       </c>
@@ -1641,11 +2234,26 @@
       <c r="D43" t="b">
         <v>0</v>
       </c>
+      <c r="E43">
+        <v>40</v>
+      </c>
       <c r="F43" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G43">
+        <v>22</v>
+      </c>
+      <c r="H43">
+        <v>92</v>
+      </c>
+      <c r="I43">
+        <v>25</v>
+      </c>
+      <c r="J43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>62</v>
       </c>
@@ -1658,11 +2266,26 @@
       <c r="D44" t="b">
         <v>1</v>
       </c>
+      <c r="E44">
+        <v>44</v>
+      </c>
       <c r="F44" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G44">
+        <v>26</v>
+      </c>
+      <c r="H44">
+        <v>99</v>
+      </c>
+      <c r="I44">
+        <v>80</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>62</v>
       </c>
@@ -1675,11 +2298,26 @@
       <c r="D45" t="b">
         <v>0</v>
       </c>
+      <c r="E45">
+        <v>4</v>
+      </c>
       <c r="F45" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G45">
+        <v>27</v>
+      </c>
+      <c r="H45">
+        <v>100</v>
+      </c>
+      <c r="I45">
+        <v>76</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>62</v>
       </c>
@@ -1692,11 +2330,26 @@
       <c r="D46" t="b">
         <v>0</v>
       </c>
+      <c r="E46">
+        <v>56</v>
+      </c>
       <c r="F46" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G46">
+        <v>24</v>
+      </c>
+      <c r="H46">
+        <v>68</v>
+      </c>
+      <c r="I46">
+        <v>67</v>
+      </c>
+      <c r="J46">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>62</v>
       </c>
@@ -1709,11 +2362,26 @@
       <c r="D47" t="b">
         <v>0</v>
       </c>
+      <c r="E47">
+        <v>38</v>
+      </c>
       <c r="F47" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G47">
+        <v>23</v>
+      </c>
+      <c r="H47">
+        <v>64</v>
+      </c>
+      <c r="I47">
+        <v>21</v>
+      </c>
+      <c r="J47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>62</v>
       </c>
@@ -1726,11 +2394,26 @@
       <c r="D48" t="b">
         <v>0</v>
       </c>
+      <c r="E48">
+        <v>46</v>
+      </c>
       <c r="F48" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G48">
+        <v>24</v>
+      </c>
+      <c r="H48">
+        <v>54</v>
+      </c>
+      <c r="I48">
+        <v>44</v>
+      </c>
+      <c r="J48">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>62</v>
       </c>
@@ -1743,8 +2426,23 @@
       <c r="D49" t="b">
         <v>0</v>
       </c>
+      <c r="E49">
+        <v>35</v>
+      </c>
       <c r="F49" s="1" t="s">
         <v>146</v>
+      </c>
+      <c r="G49">
+        <v>22</v>
+      </c>
+      <c r="H49">
+        <v>28</v>
+      </c>
+      <c r="I49">
+        <v>62</v>
+      </c>
+      <c r="J49">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add sorting functionality to player stats; implement sort controls and update rendering logic for improved user experience.
</commit_message>
<xml_diff>
--- a/templates/rosters.xlsx
+++ b/templates/rosters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c420bd46a5738fd/Documents/GitHub/nbcml/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{98E44900-1AF4-41E7-83DA-86A15D56D0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11EA5999-4B5E-42F7-9AA8-5F69EAAA0225}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{98E44900-1AF4-41E7-83DA-86A15D56D0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3254AC6C-7919-436A-9978-6E7D656C3478}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9077D6FF-DD53-4FA0-A1AB-BC2E9F42BF0A}"/>
   </bookViews>
@@ -869,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B089AB-C826-4619-B243-5B13AFD7DC37}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1735,7 +1735,7 @@
         <v>58</v>
       </c>
       <c r="I27">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="J27">
         <v>5</v>
@@ -2023,10 +2023,10 @@
         <v>83</v>
       </c>
       <c r="I36">
-        <v>73</v>
+        <v>23</v>
       </c>
       <c r="J36">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update rosters spreadsheet with latest player data
</commit_message>
<xml_diff>
--- a/templates/rosters.xlsx
+++ b/templates/rosters.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c420bd46a5738fd/Documents/GitHub/nbcml/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{98E44900-1AF4-41E7-83DA-86A15D56D0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3254AC6C-7919-436A-9978-6E7D656C3478}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{98E44900-1AF4-41E7-83DA-86A15D56D0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8739E8C1-A9AA-4570-9BD4-CF04EE84F03D}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9077D6FF-DD53-4FA0-A1AB-BC2E9F42BF0A}"/>
   </bookViews>
   <sheets>
     <sheet name="rosters" sheetId="1" r:id="rId1"/>
+    <sheet name="teams" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="151">
   <si>
     <t>Team</t>
   </si>
@@ -869,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B089AB-C826-4619-B243-5B13AFD7DC37}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -960,6 +961,9 @@
       <c r="D3" t="b">
         <v>0</v>
       </c>
+      <c r="E3">
+        <v>69</v>
+      </c>
       <c r="F3" s="1" t="s">
         <v>27</v>
       </c>
@@ -1275,6 +1279,9 @@
         <v>50</v>
       </c>
       <c r="D13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13">
         <v>0</v>
       </c>
       <c r="F13" s="1" t="s">
@@ -2450,4 +2457,24 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFDA593B-70CA-4B35-A8AE-58F429AF5E66}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add initial games data CSV file with match details for the season
</commit_message>
<xml_diff>
--- a/templates/rosters.xlsx
+++ b/templates/rosters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c420bd46a5738fd/Documents/GitHub/nbcml/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{98E44900-1AF4-41E7-83DA-86A15D56D0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8739E8C1-A9AA-4570-9BD4-CF04EE84F03D}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{98E44900-1AF4-41E7-83DA-86A15D56D0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E23741FC-549D-4869-A8AE-C5A07452AB07}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9077D6FF-DD53-4FA0-A1AB-BC2E9F42BF0A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{9077D6FF-DD53-4FA0-A1AB-BC2E9F42BF0A}"/>
   </bookViews>
   <sheets>
     <sheet name="rosters" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="166">
   <si>
     <t>Team</t>
   </si>
@@ -490,6 +490,51 @@
   </si>
   <si>
     <t>TotalTechs</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>EarlyHomeTeam</t>
+  </si>
+  <si>
+    <t>EarlyHomeScore</t>
+  </si>
+  <si>
+    <t>EarlyAwayTeam</t>
+  </si>
+  <si>
+    <t>EarlyAwayScore</t>
+  </si>
+  <si>
+    <t>MidHomeTeam</t>
+  </si>
+  <si>
+    <t>MidHomeScore</t>
+  </si>
+  <si>
+    <t>MidAwayTeam</t>
+  </si>
+  <si>
+    <t>MidAwayScore</t>
+  </si>
+  <si>
+    <t>LateHomeTeam</t>
+  </si>
+  <si>
+    <t>LateHomeScore</t>
+  </si>
+  <si>
+    <t>LateAwayTeam</t>
+  </si>
+  <si>
+    <t>LateAwayScore</t>
+  </si>
+  <si>
+    <t>06-04-2025</t>
   </si>
 </sst>
 </file>
@@ -870,7 +915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B089AB-C826-4619-B243-5B13AFD7DC37}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -2461,17 +2506,116 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFDA593B-70CA-4B35-A8AE-58F429AF5E66}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.26953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="B1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H1" t="s">
+        <v>158</v>
+      </c>
+      <c r="I1" t="s">
+        <v>159</v>
+      </c>
+      <c r="J1" t="s">
+        <v>160</v>
+      </c>
+      <c r="K1" t="s">
+        <v>161</v>
+      </c>
+      <c r="L1" t="s">
+        <v>162</v>
+      </c>
+      <c r="M1" t="s">
+        <v>163</v>
+      </c>
+      <c r="N1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>76</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2">
+        <v>70</v>
+      </c>
+      <c r="G2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2">
+        <v>90</v>
+      </c>
+      <c r="I2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2">
+        <v>94</v>
+      </c>
+      <c r="K2" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2">
+        <v>55</v>
+      </c>
+      <c r="M2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N2">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update games data CSV with complete match schedule and add new roster spreadsheet
</commit_message>
<xml_diff>
--- a/templates/rosters.xlsx
+++ b/templates/rosters.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c420bd46a5738fd/Documents/GitHub/nbcml/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{98E44900-1AF4-41E7-83DA-86A15D56D0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E23741FC-549D-4869-A8AE-C5A07452AB07}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{98E44900-1AF4-41E7-83DA-86A15D56D0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1792BF01-090E-4157-A132-C330047026A5}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{9077D6FF-DD53-4FA0-A1AB-BC2E9F42BF0A}"/>
   </bookViews>
   <sheets>
     <sheet name="rosters" sheetId="1" r:id="rId1"/>
-    <sheet name="teams" sheetId="2" r:id="rId2"/>
+    <sheet name="games" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="201">
   <si>
     <t>Team</t>
   </si>
@@ -534,7 +534,112 @@
     <t>LateAwayScore</t>
   </si>
   <si>
-    <t>06-04-2025</t>
+    <t>06-03-2025</t>
+  </si>
+  <si>
+    <t>06-10-2025</t>
+  </si>
+  <si>
+    <t>06-17-2025</t>
+  </si>
+  <si>
+    <t>06-24-2025</t>
+  </si>
+  <si>
+    <t>07-01-2025</t>
+  </si>
+  <si>
+    <t>05-13-2025</t>
+  </si>
+  <si>
+    <t>05-20-2025</t>
+  </si>
+  <si>
+    <t>05-27-2025</t>
+  </si>
+  <si>
+    <t>07-08-2025</t>
+  </si>
+  <si>
+    <t>07-15-2025</t>
+  </si>
+  <si>
+    <t>07-22-2025</t>
+  </si>
+  <si>
+    <t>07-29-2025</t>
+  </si>
+  <si>
+    <t>08-05-2025</t>
+  </si>
+  <si>
+    <t>08-12-2025</t>
+  </si>
+  <si>
+    <t>08-19-2025</t>
+  </si>
+  <si>
+    <t>08-26-2025</t>
+  </si>
+  <si>
+    <t>09-02-2025</t>
+  </si>
+  <si>
+    <t>09-09-2025</t>
+  </si>
+  <si>
+    <t>09-16-2025</t>
+  </si>
+  <si>
+    <t>09-23-2025</t>
+  </si>
+  <si>
+    <t>09-30-2025</t>
+  </si>
+  <si>
+    <t>10-07-2025</t>
+  </si>
+  <si>
+    <t>10-14-2025</t>
+  </si>
+  <si>
+    <t>10-21-2025</t>
+  </si>
+  <si>
+    <t>10-28-2025</t>
+  </si>
+  <si>
+    <t>11-04-2025</t>
+  </si>
+  <si>
+    <t>11-11-2025</t>
+  </si>
+  <si>
+    <t>11-18-2025</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>05-06-2025</t>
+  </si>
+  <si>
+    <t>11-25-2025</t>
+  </si>
+  <si>
+    <t>12-02-2025</t>
+  </si>
+  <si>
+    <t>12-09-2025</t>
   </si>
 </sst>
 </file>
@@ -576,9 +681,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2506,119 +2613,1008 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFDA593B-70CA-4B35-A8AE-58F429AF5E66}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.36328125" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>151</v>
       </c>
       <c r="B1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" t="s">
         <v>152</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>153</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>154</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>155</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>156</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>157</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>158</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>159</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>160</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>161</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>162</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>163</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>76</v>
+      </c>
+      <c r="F3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3">
+        <v>70</v>
+      </c>
+      <c r="H3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3">
+        <v>90</v>
+      </c>
+      <c r="J3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K3">
+        <v>94</v>
+      </c>
+      <c r="L3" t="s">
+        <v>61</v>
+      </c>
+      <c r="M3">
+        <v>55</v>
+      </c>
+      <c r="N3" t="s">
+        <v>62</v>
+      </c>
+      <c r="O3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4">
+        <v>53</v>
+      </c>
+      <c r="F4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4">
+        <v>65</v>
+      </c>
+      <c r="H4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4">
+        <v>85</v>
+      </c>
+      <c r="J4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K4">
+        <v>90</v>
+      </c>
+      <c r="L4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <v>66</v>
+      </c>
+      <c r="N4" t="s">
+        <v>61</v>
+      </c>
+      <c r="O4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5">
+        <v>78</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>80</v>
+      </c>
+      <c r="H5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I5">
+        <v>67</v>
+      </c>
+      <c r="J5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K5">
+        <v>78</v>
+      </c>
+      <c r="L5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5">
+        <v>56</v>
+      </c>
+      <c r="N5" t="s">
+        <v>62</v>
+      </c>
+      <c r="O5">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2">
+      <c r="D6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6">
+        <v>66</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6">
+        <v>58</v>
+      </c>
+      <c r="H6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I6">
         <v>76</v>
       </c>
-      <c r="E2" t="s">
+      <c r="J6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>78</v>
+      </c>
+      <c r="L6" t="s">
+        <v>59</v>
+      </c>
+      <c r="M6">
+        <v>79</v>
+      </c>
+      <c r="N6" t="s">
+        <v>61</v>
+      </c>
+      <c r="O6">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>194</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" t="s">
+        <v>61</v>
+      </c>
+      <c r="J7" t="s">
         <v>34</v>
       </c>
-      <c r="F2">
-        <v>70</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="L7" t="s">
+        <v>62</v>
+      </c>
+      <c r="N7" t="s">
         <v>59</v>
       </c>
-      <c r="H2">
-        <v>90</v>
-      </c>
-      <c r="I2" t="s">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" t="s">
         <v>60</v>
       </c>
-      <c r="J2">
-        <v>94</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="J8" t="s">
+        <v>59</v>
+      </c>
+      <c r="L8" t="s">
         <v>61</v>
       </c>
-      <c r="L2">
-        <v>55</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="N8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>194</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" t="s">
         <v>62</v>
       </c>
-      <c r="N2">
-        <v>50</v>
+      <c r="L9" t="s">
+        <v>60</v>
+      </c>
+      <c r="N9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>194</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" t="s">
+        <v>62</v>
+      </c>
+      <c r="J10" t="s">
+        <v>61</v>
+      </c>
+      <c r="L10" t="s">
+        <v>4</v>
+      </c>
+      <c r="N10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11" t="s">
+        <v>61</v>
+      </c>
+      <c r="L11" t="s">
+        <v>59</v>
+      </c>
+      <c r="N11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>194</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" t="s">
+        <v>59</v>
+      </c>
+      <c r="L12" t="s">
+        <v>60</v>
+      </c>
+      <c r="N12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>194</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J13" t="s">
+        <v>62</v>
+      </c>
+      <c r="L13" t="s">
+        <v>59</v>
+      </c>
+      <c r="N13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>194</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H14" t="s">
+        <v>59</v>
+      </c>
+      <c r="J14" t="s">
+        <v>34</v>
+      </c>
+      <c r="L14" t="s">
+        <v>62</v>
+      </c>
+      <c r="N14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>194</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" t="s">
+        <v>62</v>
+      </c>
+      <c r="H15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J15" t="s">
+        <v>4</v>
+      </c>
+      <c r="L15" t="s">
+        <v>61</v>
+      </c>
+      <c r="N15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>194</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16" t="s">
+        <v>62</v>
+      </c>
+      <c r="J16" t="s">
+        <v>34</v>
+      </c>
+      <c r="L16" t="s">
+        <v>4</v>
+      </c>
+      <c r="N16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>194</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" t="s">
+        <v>4</v>
+      </c>
+      <c r="J17" t="s">
+        <v>60</v>
+      </c>
+      <c r="L17" t="s">
+        <v>62</v>
+      </c>
+      <c r="N17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>194</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" t="s">
+        <v>61</v>
+      </c>
+      <c r="H18" t="s">
+        <v>59</v>
+      </c>
+      <c r="J18" t="s">
+        <v>62</v>
+      </c>
+      <c r="L18" t="s">
+        <v>34</v>
+      </c>
+      <c r="N18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>194</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>59</v>
+      </c>
+      <c r="H19" t="s">
+        <v>61</v>
+      </c>
+      <c r="J19" t="s">
+        <v>60</v>
+      </c>
+      <c r="L19" t="s">
+        <v>34</v>
+      </c>
+      <c r="N19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>194</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" t="s">
+        <v>34</v>
+      </c>
+      <c r="J20" t="s">
+        <v>61</v>
+      </c>
+      <c r="L20" t="s">
+        <v>60</v>
+      </c>
+      <c r="N20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>194</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D21" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21" t="s">
+        <v>61</v>
+      </c>
+      <c r="H21" t="s">
+        <v>60</v>
+      </c>
+      <c r="J21" t="s">
+        <v>34</v>
+      </c>
+      <c r="L21" t="s">
+        <v>4</v>
+      </c>
+      <c r="N21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>194</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" t="s">
+        <v>59</v>
+      </c>
+      <c r="H22" t="s">
+        <v>62</v>
+      </c>
+      <c r="J22" t="s">
+        <v>60</v>
+      </c>
+      <c r="L22" t="s">
+        <v>61</v>
+      </c>
+      <c r="N22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>194</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H23" t="s">
+        <v>60</v>
+      </c>
+      <c r="J23" t="s">
+        <v>62</v>
+      </c>
+      <c r="L23" t="s">
+        <v>59</v>
+      </c>
+      <c r="N23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>194</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D24" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" t="s">
+        <v>62</v>
+      </c>
+      <c r="H24" t="s">
+        <v>59</v>
+      </c>
+      <c r="J24" t="s">
+        <v>4</v>
+      </c>
+      <c r="L24" t="s">
+        <v>34</v>
+      </c>
+      <c r="N24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>194</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D25" t="s">
+        <v>60</v>
+      </c>
+      <c r="F25" t="s">
+        <v>59</v>
+      </c>
+      <c r="H25" t="s">
+        <v>4</v>
+      </c>
+      <c r="J25" t="s">
+        <v>61</v>
+      </c>
+      <c r="L25" t="s">
+        <v>62</v>
+      </c>
+      <c r="N25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>194</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D26" t="s">
+        <v>34</v>
+      </c>
+      <c r="F26" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26" t="s">
+        <v>61</v>
+      </c>
+      <c r="J26" t="s">
+        <v>59</v>
+      </c>
+      <c r="L26" t="s">
+        <v>60</v>
+      </c>
+      <c r="N26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>194</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D27" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" t="s">
+        <v>61</v>
+      </c>
+      <c r="H27" t="s">
+        <v>60</v>
+      </c>
+      <c r="J27" t="s">
+        <v>4</v>
+      </c>
+      <c r="L27" t="s">
+        <v>34</v>
+      </c>
+      <c r="N27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>194</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D28" t="s">
+        <v>59</v>
+      </c>
+      <c r="F28" t="s">
+        <v>34</v>
+      </c>
+      <c r="H28" t="s">
+        <v>4</v>
+      </c>
+      <c r="J28" t="s">
+        <v>62</v>
+      </c>
+      <c r="L28" t="s">
+        <v>61</v>
+      </c>
+      <c r="N28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>194</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D29" t="s">
+        <v>61</v>
+      </c>
+      <c r="F29" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29" t="s">
+        <v>62</v>
+      </c>
+      <c r="J29" t="s">
+        <v>59</v>
+      </c>
+      <c r="L29" t="s">
+        <v>4</v>
+      </c>
+      <c r="N29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>194</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F30" t="s">
+        <v>61</v>
+      </c>
+      <c r="H30" t="s">
+        <v>34</v>
+      </c>
+      <c r="J30" t="s">
+        <v>62</v>
+      </c>
+      <c r="L30" t="s">
+        <v>59</v>
+      </c>
+      <c r="N30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>195</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>195</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>195</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove outdated player statistics from data store and update rosters spreadsheet with new player information
</commit_message>
<xml_diff>
--- a/templates/rosters.xlsx
+++ b/templates/rosters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c420bd46a5738fd/Documents/GitHub/nbcml/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{98E44900-1AF4-41E7-83DA-86A15D56D0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1792BF01-090E-4157-A132-C330047026A5}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{98E44900-1AF4-41E7-83DA-86A15D56D0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C28A29C0-D6CC-4485-8977-F6891C02347B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{9077D6FF-DD53-4FA0-A1AB-BC2E9F42BF0A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="210">
   <si>
     <t>Team</t>
   </si>
@@ -640,6 +640,33 @@
   </si>
   <si>
     <t>12-09-2025</t>
+  </si>
+  <si>
+    <t>EarlySK1</t>
+  </si>
+  <si>
+    <t>EarlySK2</t>
+  </si>
+  <si>
+    <t>MidSK1</t>
+  </si>
+  <si>
+    <t>MidSk2</t>
+  </si>
+  <si>
+    <t>LateSK1</t>
+  </si>
+  <si>
+    <t>LateSK2</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>12-16-2025</t>
+  </si>
+  <si>
+    <t>12-23-2025</t>
   </si>
 </sst>
 </file>
@@ -681,11 +708,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2613,10 +2639,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFDA593B-70CA-4B35-A8AE-58F429AF5E66}">
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="T30" sqref="T30:U32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2628,17 +2654,19 @@
     <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.6328125" customWidth="1"/>
+    <col min="10" max="10" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="12.54296875" customWidth="1"/>
+    <col min="16" max="16" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>151</v>
       </c>
@@ -2661,31 +2689,49 @@
         <v>156</v>
       </c>
       <c r="H1" t="s">
+        <v>201</v>
+      </c>
+      <c r="I1" t="s">
+        <v>202</v>
+      </c>
+      <c r="J1" t="s">
         <v>157</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>158</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>159</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>160</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
+        <v>203</v>
+      </c>
+      <c r="O1" t="s">
+        <v>204</v>
+      </c>
+      <c r="P1" t="s">
         <v>161</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Q1" t="s">
         <v>162</v>
       </c>
-      <c r="N1" t="s">
+      <c r="R1" t="s">
         <v>163</v>
       </c>
-      <c r="O1" t="s">
+      <c r="S1" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="T1" t="s">
+        <v>205</v>
+      </c>
+      <c r="U1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2696,14 +2742,14 @@
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>194</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>170</v>
       </c>
       <c r="D3" t="s">
@@ -2719,38 +2765,56 @@
         <v>70</v>
       </c>
       <c r="H3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>88</v>
+      </c>
+      <c r="J3" t="s">
         <v>59</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>90</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>60</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>94</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" t="s">
+        <v>119</v>
+      </c>
+      <c r="P3" t="s">
         <v>61</v>
       </c>
-      <c r="M3">
+      <c r="Q3">
         <v>55</v>
       </c>
-      <c r="N3" t="s">
+      <c r="R3" t="s">
         <v>62</v>
       </c>
-      <c r="O3">
+      <c r="S3">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="T3" t="s">
+        <v>43</v>
+      </c>
+      <c r="U3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>171</v>
       </c>
       <c r="D4" t="s">
@@ -2766,38 +2830,56 @@
         <v>65</v>
       </c>
       <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" t="s">
+        <v>90</v>
+      </c>
+      <c r="J4" t="s">
         <v>34</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>85</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>59</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <v>90</v>
       </c>
-      <c r="L4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M4">
+      <c r="N4" t="s">
         <v>66</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
+        <v>78</v>
+      </c>
+      <c r="P4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q4">
+        <v>66</v>
+      </c>
+      <c r="R4" t="s">
         <v>61</v>
       </c>
-      <c r="O4">
+      <c r="S4">
         <v>71</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="T4" t="s">
+        <v>45</v>
+      </c>
+      <c r="U4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>194</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>172</v>
       </c>
       <c r="D5" t="s">
@@ -2813,38 +2895,56 @@
         <v>80</v>
       </c>
       <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="s">
+        <v>92</v>
+      </c>
+      <c r="J5" t="s">
         <v>61</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>67</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>60</v>
       </c>
-      <c r="K5">
+      <c r="M5">
         <v>78</v>
       </c>
-      <c r="L5" t="s">
+      <c r="N5" t="s">
+        <v>68</v>
+      </c>
+      <c r="O5" t="s">
+        <v>86</v>
+      </c>
+      <c r="P5" t="s">
         <v>34</v>
       </c>
-      <c r="M5">
+      <c r="Q5">
         <v>56</v>
       </c>
-      <c r="N5" t="s">
+      <c r="R5" t="s">
         <v>62</v>
       </c>
-      <c r="O5">
+      <c r="S5">
         <v>82</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="T5" t="s">
+        <v>47</v>
+      </c>
+      <c r="U5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>194</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>165</v>
       </c>
       <c r="D6" t="s">
@@ -2860,31 +2960,49 @@
         <v>58</v>
       </c>
       <c r="H6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" t="s">
+        <v>94</v>
+      </c>
+      <c r="J6" t="s">
         <v>62</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>76</v>
       </c>
-      <c r="J6" t="s">
-        <v>4</v>
-      </c>
-      <c r="K6">
+      <c r="L6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6">
         <v>78</v>
       </c>
-      <c r="L6" t="s">
+      <c r="N6" t="s">
+        <v>70</v>
+      </c>
+      <c r="O6" t="s">
+        <v>10</v>
+      </c>
+      <c r="P6" t="s">
         <v>59</v>
       </c>
-      <c r="M6">
+      <c r="Q6">
         <v>79</v>
       </c>
-      <c r="N6" t="s">
+      <c r="R6" t="s">
         <v>61</v>
       </c>
-      <c r="O6">
+      <c r="S6">
         <v>73</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="T6" t="s">
+        <v>49</v>
+      </c>
+      <c r="U6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2901,19 +3019,37 @@
         <v>60</v>
       </c>
       <c r="H7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J7" t="s">
         <v>61</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>34</v>
       </c>
-      <c r="L7" t="s">
+      <c r="N7" t="s">
+        <v>72</v>
+      </c>
+      <c r="O7" t="s">
+        <v>12</v>
+      </c>
+      <c r="P7" t="s">
         <v>62</v>
       </c>
-      <c r="N7" t="s">
+      <c r="R7" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="T7" t="s">
+        <v>51</v>
+      </c>
+      <c r="U7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2930,19 +3066,37 @@
         <v>62</v>
       </c>
       <c r="H8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" t="s">
+        <v>97</v>
+      </c>
+      <c r="J8" t="s">
         <v>60</v>
       </c>
-      <c r="J8" t="s">
+      <c r="L8" t="s">
         <v>59</v>
       </c>
-      <c r="L8" t="s">
+      <c r="N8" t="s">
+        <v>74</v>
+      </c>
+      <c r="O8" t="s">
+        <v>14</v>
+      </c>
+      <c r="P8" t="s">
         <v>61</v>
       </c>
-      <c r="N8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="R8" t="s">
+        <v>4</v>
+      </c>
+      <c r="T8" t="s">
+        <v>53</v>
+      </c>
+      <c r="U8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2959,19 +3113,37 @@
         <v>59</v>
       </c>
       <c r="H9" t="s">
-        <v>4</v>
+        <v>22</v>
+      </c>
+      <c r="I9" t="s">
+        <v>99</v>
       </c>
       <c r="J9" t="s">
+        <v>4</v>
+      </c>
+      <c r="L9" t="s">
         <v>62</v>
       </c>
-      <c r="L9" t="s">
+      <c r="N9" t="s">
+        <v>9</v>
+      </c>
+      <c r="O9" t="s">
+        <v>16</v>
+      </c>
+      <c r="P9" t="s">
         <v>60</v>
       </c>
-      <c r="N9" t="s">
+      <c r="R9" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="T9" t="s">
+        <v>55</v>
+      </c>
+      <c r="U9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2988,48 +3160,48 @@
         <v>34</v>
       </c>
       <c r="H10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" t="s">
+        <v>101</v>
+      </c>
+      <c r="J10" t="s">
         <v>62</v>
       </c>
-      <c r="J10" t="s">
+      <c r="L10" t="s">
         <v>61</v>
       </c>
-      <c r="L10" t="s">
-        <v>4</v>
-      </c>
       <c r="N10" t="s">
+        <v>77</v>
+      </c>
+      <c r="O10" t="s">
+        <v>18</v>
+      </c>
+      <c r="P10" t="s">
+        <v>4</v>
+      </c>
+      <c r="R10" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="T10" t="s">
+        <v>57</v>
+      </c>
+      <c r="U10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>194</v>
+        <v>207</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="D11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" t="s">
-        <v>34</v>
-      </c>
-      <c r="J11" t="s">
-        <v>61</v>
-      </c>
-      <c r="L11" t="s">
-        <v>59</v>
-      </c>
-      <c r="N11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3040,25 +3212,43 @@
         <v>174</v>
       </c>
       <c r="D12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" t="s">
+        <v>103</v>
+      </c>
+      <c r="J12" t="s">
+        <v>34</v>
+      </c>
+      <c r="L12" t="s">
+        <v>61</v>
+      </c>
+      <c r="N12" t="s">
+        <v>79</v>
+      </c>
+      <c r="O12" t="s">
+        <v>20</v>
+      </c>
+      <c r="P12" t="s">
+        <v>59</v>
+      </c>
+      <c r="R12" t="s">
         <v>62</v>
       </c>
-      <c r="F12" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J12" t="s">
-        <v>59</v>
-      </c>
-      <c r="L12" t="s">
-        <v>60</v>
-      </c>
-      <c r="N12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="T12" t="s">
+        <v>63</v>
+      </c>
+      <c r="U12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3069,25 +3259,43 @@
         <v>175</v>
       </c>
       <c r="D13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" t="s">
         <v>34</v>
       </c>
-      <c r="F13" t="s">
-        <v>60</v>
-      </c>
       <c r="H13" t="s">
-        <v>61</v>
+        <v>45</v>
+      </c>
+      <c r="I13" t="s">
+        <v>105</v>
       </c>
       <c r="J13" t="s">
-        <v>62</v>
+        <v>4</v>
       </c>
       <c r="L13" t="s">
         <v>59</v>
       </c>
       <c r="N13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+      <c r="O13" t="s">
+        <v>22</v>
+      </c>
+      <c r="P13" t="s">
+        <v>60</v>
+      </c>
+      <c r="R13" t="s">
+        <v>61</v>
+      </c>
+      <c r="T13" t="s">
+        <v>7</v>
+      </c>
+      <c r="U13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3098,25 +3306,43 @@
         <v>176</v>
       </c>
       <c r="D14" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="F14" t="s">
+        <v>60</v>
+      </c>
+      <c r="H14" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" t="s">
+        <v>107</v>
+      </c>
+      <c r="J14" t="s">
         <v>61</v>
-      </c>
-      <c r="H14" t="s">
-        <v>59</v>
-      </c>
-      <c r="J14" t="s">
-        <v>34</v>
       </c>
       <c r="L14" t="s">
         <v>62</v>
       </c>
       <c r="N14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+      <c r="O14" t="s">
+        <v>24</v>
+      </c>
+      <c r="P14" t="s">
+        <v>59</v>
+      </c>
+      <c r="R14" t="s">
+        <v>4</v>
+      </c>
+      <c r="T14" t="s">
+        <v>66</v>
+      </c>
+      <c r="U14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3127,25 +3353,43 @@
         <v>177</v>
       </c>
       <c r="D15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>61</v>
+      </c>
+      <c r="H15" t="s">
+        <v>49</v>
+      </c>
+      <c r="I15" t="s">
+        <v>109</v>
+      </c>
+      <c r="J15" t="s">
+        <v>59</v>
+      </c>
+      <c r="L15" t="s">
+        <v>34</v>
+      </c>
+      <c r="N15" t="s">
+        <v>10</v>
+      </c>
+      <c r="O15" t="s">
+        <v>88</v>
+      </c>
+      <c r="P15" t="s">
+        <v>62</v>
+      </c>
+      <c r="R15" t="s">
         <v>60</v>
       </c>
-      <c r="F15" t="s">
-        <v>62</v>
-      </c>
-      <c r="H15" t="s">
-        <v>34</v>
-      </c>
-      <c r="J15" t="s">
-        <v>4</v>
-      </c>
-      <c r="L15" t="s">
-        <v>61</v>
-      </c>
-      <c r="N15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="T15" t="s">
+        <v>68</v>
+      </c>
+      <c r="U15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3156,13 +3400,16 @@
         <v>178</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F16" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H16" t="s">
-        <v>62</v>
+        <v>51</v>
+      </c>
+      <c r="I16" t="s">
+        <v>109</v>
       </c>
       <c r="J16" t="s">
         <v>34</v>
@@ -3171,10 +3418,25 @@
         <v>4</v>
       </c>
       <c r="N16" t="s">
+        <v>12</v>
+      </c>
+      <c r="O16" t="s">
+        <v>90</v>
+      </c>
+      <c r="P16" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="R16" t="s">
+        <v>59</v>
+      </c>
+      <c r="T16" t="s">
+        <v>70</v>
+      </c>
+      <c r="U16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3185,25 +3447,43 @@
         <v>179</v>
       </c>
       <c r="D17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" t="s">
+        <v>60</v>
+      </c>
+      <c r="H17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I17" t="s">
+        <v>112</v>
+      </c>
+      <c r="J17" t="s">
+        <v>62</v>
+      </c>
+      <c r="L17" t="s">
+        <v>34</v>
+      </c>
+      <c r="N17" t="s">
+        <v>14</v>
+      </c>
+      <c r="O17" t="s">
+        <v>92</v>
+      </c>
+      <c r="P17" t="s">
+        <v>4</v>
+      </c>
+      <c r="R17" t="s">
         <v>61</v>
       </c>
-      <c r="F17" t="s">
-        <v>34</v>
-      </c>
-      <c r="H17" t="s">
-        <v>4</v>
-      </c>
-      <c r="J17" t="s">
-        <v>60</v>
-      </c>
-      <c r="L17" t="s">
-        <v>62</v>
-      </c>
-      <c r="N17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="T17" t="s">
+        <v>72</v>
+      </c>
+      <c r="U17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3214,25 +3494,43 @@
         <v>180</v>
       </c>
       <c r="D18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" t="s">
+        <v>55</v>
+      </c>
+      <c r="I18" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" t="s">
+        <v>4</v>
+      </c>
+      <c r="L18" t="s">
         <v>60</v>
       </c>
-      <c r="F18" t="s">
-        <v>61</v>
-      </c>
-      <c r="H18" t="s">
+      <c r="N18" t="s">
+        <v>16</v>
+      </c>
+      <c r="O18" t="s">
+        <v>94</v>
+      </c>
+      <c r="P18" t="s">
+        <v>62</v>
+      </c>
+      <c r="R18" t="s">
         <v>59</v>
       </c>
-      <c r="J18" t="s">
-        <v>62</v>
-      </c>
-      <c r="L18" t="s">
-        <v>34</v>
-      </c>
-      <c r="N18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="T18" t="s">
+        <v>74</v>
+      </c>
+      <c r="U18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3243,25 +3541,43 @@
         <v>181</v>
       </c>
       <c r="D19" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="F19" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" t="s">
+        <v>57</v>
+      </c>
+      <c r="I19" t="s">
+        <v>115</v>
+      </c>
+      <c r="J19" t="s">
         <v>59</v>
       </c>
-      <c r="H19" t="s">
-        <v>61</v>
-      </c>
-      <c r="J19" t="s">
-        <v>60</v>
-      </c>
       <c r="L19" t="s">
+        <v>62</v>
+      </c>
+      <c r="N19" t="s">
+        <v>18</v>
+      </c>
+      <c r="O19" t="s">
+        <v>88</v>
+      </c>
+      <c r="P19" t="s">
         <v>34</v>
       </c>
-      <c r="N19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="R19" t="s">
+        <v>4</v>
+      </c>
+      <c r="T19" t="s">
+        <v>9</v>
+      </c>
+      <c r="U19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3272,13 +3588,16 @@
         <v>182</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>4</v>
       </c>
       <c r="F20" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="H20" t="s">
-        <v>34</v>
+        <v>63</v>
+      </c>
+      <c r="I20" t="s">
+        <v>117</v>
       </c>
       <c r="J20" t="s">
         <v>61</v>
@@ -3287,39 +3606,36 @@
         <v>60</v>
       </c>
       <c r="N20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="O20" t="s">
+        <v>97</v>
+      </c>
+      <c r="P20" t="s">
+        <v>34</v>
+      </c>
+      <c r="R20" t="s">
+        <v>62</v>
+      </c>
+      <c r="T20" t="s">
+        <v>77</v>
+      </c>
+      <c r="U20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>194</v>
+        <v>207</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D21" t="s">
-        <v>59</v>
-      </c>
-      <c r="F21" t="s">
-        <v>61</v>
-      </c>
-      <c r="H21" t="s">
-        <v>60</v>
-      </c>
-      <c r="J21" t="s">
-        <v>34</v>
-      </c>
-      <c r="L21" t="s">
-        <v>4</v>
-      </c>
-      <c r="N21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3330,25 +3646,43 @@
         <v>184</v>
       </c>
       <c r="D22" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" t="s">
+        <v>119</v>
+      </c>
+      <c r="J22" t="s">
         <v>34</v>
-      </c>
-      <c r="F22" t="s">
-        <v>59</v>
-      </c>
-      <c r="H22" t="s">
-        <v>62</v>
-      </c>
-      <c r="J22" t="s">
-        <v>60</v>
       </c>
       <c r="L22" t="s">
         <v>61</v>
       </c>
       <c r="N22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+      <c r="O22" t="s">
+        <v>99</v>
+      </c>
+      <c r="P22" t="s">
+        <v>60</v>
+      </c>
+      <c r="R22" t="s">
+        <v>59</v>
+      </c>
+      <c r="T22" t="s">
+        <v>10</v>
+      </c>
+      <c r="U22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3359,25 +3693,43 @@
         <v>185</v>
       </c>
       <c r="D23" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="F23" t="s">
+        <v>61</v>
+      </c>
+      <c r="H23" t="s">
+        <v>66</v>
+      </c>
+      <c r="I23" t="s">
+        <v>78</v>
+      </c>
+      <c r="J23" t="s">
+        <v>60</v>
+      </c>
+      <c r="L23" t="s">
         <v>34</v>
       </c>
-      <c r="H23" t="s">
-        <v>60</v>
-      </c>
-      <c r="J23" t="s">
+      <c r="N23" t="s">
+        <v>24</v>
+      </c>
+      <c r="O23" t="s">
+        <v>101</v>
+      </c>
+      <c r="P23" t="s">
+        <v>4</v>
+      </c>
+      <c r="R23" t="s">
         <v>62</v>
       </c>
-      <c r="L23" t="s">
-        <v>59</v>
-      </c>
-      <c r="N23" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="T23" t="s">
+        <v>12</v>
+      </c>
+      <c r="U23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3388,25 +3740,43 @@
         <v>186</v>
       </c>
       <c r="D24" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" t="s">
+        <v>59</v>
+      </c>
+      <c r="H24" t="s">
+        <v>68</v>
+      </c>
+      <c r="I24" t="s">
+        <v>86</v>
+      </c>
+      <c r="J24" t="s">
+        <v>62</v>
+      </c>
+      <c r="L24" t="s">
+        <v>60</v>
+      </c>
+      <c r="N24" t="s">
+        <v>43</v>
+      </c>
+      <c r="O24" t="s">
+        <v>103</v>
+      </c>
+      <c r="P24" t="s">
         <v>61</v>
       </c>
-      <c r="F24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H24" t="s">
-        <v>59</v>
-      </c>
-      <c r="J24" t="s">
-        <v>4</v>
-      </c>
-      <c r="L24" t="s">
-        <v>34</v>
-      </c>
-      <c r="N24" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="R24" t="s">
+        <v>4</v>
+      </c>
+      <c r="T24" t="s">
+        <v>14</v>
+      </c>
+      <c r="U24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3417,25 +3787,43 @@
         <v>187</v>
       </c>
       <c r="D25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" t="s">
+        <v>34</v>
+      </c>
+      <c r="H25" t="s">
+        <v>70</v>
+      </c>
+      <c r="I25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J25" t="s">
         <v>60</v>
-      </c>
-      <c r="F25" t="s">
-        <v>59</v>
-      </c>
-      <c r="H25" t="s">
-        <v>4</v>
-      </c>
-      <c r="J25" t="s">
-        <v>61</v>
       </c>
       <c r="L25" t="s">
         <v>62</v>
       </c>
       <c r="N25" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+      <c r="O25" t="s">
+        <v>105</v>
+      </c>
+      <c r="P25" t="s">
+        <v>59</v>
+      </c>
+      <c r="R25" t="s">
+        <v>61</v>
+      </c>
+      <c r="T25" t="s">
+        <v>16</v>
+      </c>
+      <c r="U25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3446,25 +3834,43 @@
         <v>188</v>
       </c>
       <c r="D26" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="F26" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="H26" t="s">
-        <v>61</v>
+        <v>72</v>
+      </c>
+      <c r="I26" t="s">
+        <v>12</v>
       </c>
       <c r="J26" t="s">
         <v>59</v>
       </c>
       <c r="L26" t="s">
+        <v>4</v>
+      </c>
+      <c r="N26" t="s">
+        <v>47</v>
+      </c>
+      <c r="O26" t="s">
+        <v>107</v>
+      </c>
+      <c r="P26" t="s">
+        <v>34</v>
+      </c>
+      <c r="R26" t="s">
         <v>60</v>
       </c>
-      <c r="N26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="T26" t="s">
+        <v>18</v>
+      </c>
+      <c r="U26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3475,25 +3881,43 @@
         <v>189</v>
       </c>
       <c r="D27" t="s">
+        <v>60</v>
+      </c>
+      <c r="F27" t="s">
+        <v>59</v>
+      </c>
+      <c r="H27" t="s">
+        <v>74</v>
+      </c>
+      <c r="I27" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27" t="s">
+        <v>4</v>
+      </c>
+      <c r="L27" t="s">
+        <v>61</v>
+      </c>
+      <c r="N27" t="s">
+        <v>49</v>
+      </c>
+      <c r="O27" t="s">
+        <v>109</v>
+      </c>
+      <c r="P27" t="s">
         <v>62</v>
       </c>
-      <c r="F27" t="s">
-        <v>61</v>
-      </c>
-      <c r="H27" t="s">
-        <v>60</v>
-      </c>
-      <c r="J27" t="s">
-        <v>4</v>
-      </c>
-      <c r="L27" t="s">
+      <c r="R27" t="s">
         <v>34</v>
       </c>
-      <c r="N27" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="T27" t="s">
+        <v>20</v>
+      </c>
+      <c r="U27" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3504,25 +3928,43 @@
         <v>190</v>
       </c>
       <c r="D28" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" t="s">
+        <v>4</v>
+      </c>
+      <c r="H28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I28" t="s">
+        <v>16</v>
+      </c>
+      <c r="J28" t="s">
+        <v>61</v>
+      </c>
+      <c r="L28" t="s">
         <v>59</v>
       </c>
-      <c r="F28" t="s">
-        <v>34</v>
-      </c>
-      <c r="H28" t="s">
-        <v>4</v>
-      </c>
-      <c r="J28" t="s">
+      <c r="N28" t="s">
+        <v>51</v>
+      </c>
+      <c r="O28" t="s">
+        <v>109</v>
+      </c>
+      <c r="P28" t="s">
+        <v>60</v>
+      </c>
+      <c r="R28" t="s">
         <v>62</v>
       </c>
-      <c r="L28" t="s">
-        <v>61</v>
-      </c>
-      <c r="N28" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="T28" t="s">
+        <v>22</v>
+      </c>
+      <c r="U28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3533,25 +3975,43 @@
         <v>191</v>
       </c>
       <c r="D29" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" t="s">
         <v>61</v>
       </c>
-      <c r="F29" t="s">
+      <c r="H29" t="s">
+        <v>77</v>
+      </c>
+      <c r="I29" t="s">
+        <v>18</v>
+      </c>
+      <c r="J29" t="s">
+        <v>60</v>
+      </c>
+      <c r="L29" t="s">
+        <v>4</v>
+      </c>
+      <c r="N29" t="s">
+        <v>53</v>
+      </c>
+      <c r="O29" t="s">
+        <v>112</v>
+      </c>
+      <c r="P29" t="s">
         <v>34</v>
       </c>
-      <c r="H29" t="s">
-        <v>62</v>
-      </c>
-      <c r="J29" t="s">
+      <c r="R29" t="s">
         <v>59</v>
       </c>
-      <c r="L29" t="s">
-        <v>4</v>
-      </c>
-      <c r="N29" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="T29" t="s">
+        <v>24</v>
+      </c>
+      <c r="U29" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3562,44 +4022,134 @@
         <v>192</v>
       </c>
       <c r="D30" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" t="s">
+        <v>34</v>
+      </c>
+      <c r="H30" t="s">
+        <v>79</v>
+      </c>
+      <c r="I30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J30" t="s">
+        <v>4</v>
+      </c>
+      <c r="L30" t="s">
+        <v>62</v>
+      </c>
+      <c r="N30" t="s">
+        <v>55</v>
+      </c>
+      <c r="O30" t="s">
+        <v>8</v>
+      </c>
+      <c r="P30" t="s">
+        <v>61</v>
+      </c>
+      <c r="R30" t="s">
         <v>60</v>
       </c>
-      <c r="F30" t="s">
-        <v>61</v>
-      </c>
-      <c r="H30" t="s">
-        <v>34</v>
-      </c>
-      <c r="J30" t="s">
-        <v>62</v>
-      </c>
-      <c r="L30" t="s">
-        <v>59</v>
-      </c>
-      <c r="N30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="T30" t="s">
+        <v>74</v>
+      </c>
+      <c r="U30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="D31" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" t="s">
+        <v>34</v>
+      </c>
+      <c r="H31" t="s">
+        <v>81</v>
+      </c>
+      <c r="I31" t="s">
+        <v>22</v>
+      </c>
+      <c r="J31" t="s">
+        <v>62</v>
+      </c>
+      <c r="L31" t="s">
+        <v>59</v>
+      </c>
+      <c r="N31" t="s">
+        <v>57</v>
+      </c>
+      <c r="O31" t="s">
+        <v>115</v>
+      </c>
+      <c r="P31" t="s">
+        <v>4</v>
+      </c>
+      <c r="R31" t="s">
+        <v>60</v>
+      </c>
+      <c r="T31" t="s">
+        <v>9</v>
+      </c>
+      <c r="U31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>199</v>
+      </c>
+      <c r="D32" t="s">
+        <v>60</v>
+      </c>
+      <c r="F32" t="s">
+        <v>61</v>
+      </c>
+      <c r="H32" t="s">
+        <v>83</v>
+      </c>
+      <c r="I32" t="s">
+        <v>24</v>
+      </c>
+      <c r="J32" t="s">
+        <v>34</v>
+      </c>
+      <c r="L32" t="s">
+        <v>62</v>
+      </c>
+      <c r="N32" t="s">
+        <v>63</v>
+      </c>
+      <c r="O32" t="s">
+        <v>117</v>
+      </c>
+      <c r="P32" t="s">
+        <v>59</v>
+      </c>
+      <c r="R32" t="s">
+        <v>4</v>
+      </c>
+      <c r="T32" t="s">
+        <v>77</v>
+      </c>
+      <c r="U32" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -3611,6 +4161,28 @@
       </c>
       <c r="C33" s="2" t="s">
         <v>200</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>195</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>195</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>